<commit_message>
update column type in excel
</commit_message>
<xml_diff>
--- a/calculations/calculations.xlsx
+++ b/calculations/calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\DDDD-Project\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06A3D2D-5E4C-47F4-9040-113E2996DC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3933C2C5-D203-4D1B-804D-C969B0C657AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>